<commit_message>
Saved buoy data to environmental metadata
</commit_message>
<xml_diff>
--- a/environmental_data/for_humans/bacterial_production_results.xlsx
+++ b/environmental_data/for_humans/bacterial_production_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amlin\Dropbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\geodes\environmental_data\for_humans\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="14">
   <si>
     <t>Sample #</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Averaged_result</t>
   </si>
 </sst>
 </file>
@@ -382,8 +385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H211"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G122" sqref="G122"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68:H134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,8 +413,8 @@
       <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="H1">
-        <v>19</v>
+      <c r="H1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -436,6 +439,10 @@
       <c r="G2">
         <v>60</v>
       </c>
+      <c r="H2">
+        <f>(AVERAGE(E2:E5) - AVERAGE(E6:E7)) * 60/AVERAGE(G2:G5)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -574,6 +581,10 @@
       <c r="G8">
         <v>60</v>
       </c>
+      <c r="H8">
+        <f>(AVERAGE(E8:E11) - AVERAGE(E12:E13)) * 60/AVERAGE(G8:G11)</f>
+        <v>-4.25</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -712,6 +723,10 @@
       <c r="G14">
         <v>60</v>
       </c>
+      <c r="H14">
+        <f>(AVERAGE(E14:E17) - AVERAGE(E18:E19)) * 60/AVERAGE(G14:G17)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -759,7 +774,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -782,7 +797,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -805,7 +820,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -828,7 +843,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -850,8 +865,12 @@
       <c r="G20">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <f>(AVERAGE(E20:E23) - AVERAGE(E24:E25)) * 60/AVERAGE(G20:G23)</f>
+        <v>-1.2244897959183674</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -874,7 +893,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -897,7 +916,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -920,7 +939,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -943,7 +962,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -966,7 +985,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -988,8 +1007,12 @@
       <c r="G26">
         <v>60</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <f>(AVERAGE(E26:E29) - AVERAGE(E30:E31)) * 60/AVERAGE(G26:G29)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1012,7 +1035,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1035,7 +1058,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1058,7 +1081,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1081,7 +1104,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1104,7 +1127,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1126,8 +1149,12 @@
       <c r="G32">
         <v>60</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <f>(AVERAGE(E32:E35) - AVERAGE(E36:E37)) * 60/AVERAGE(G32:G35)</f>
+        <v>5.5696202531645573</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1150,7 +1177,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1173,7 +1200,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1196,7 +1223,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1219,7 +1246,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1242,7 +1269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1264,8 +1291,12 @@
       <c r="G38">
         <v>60</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <f>(AVERAGE(E38:E41) - AVERAGE(E42:E43)) * 60/AVERAGE(G38:G41)</f>
+        <v>-1.25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1288,7 +1319,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1311,7 +1342,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1334,7 +1365,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1357,7 +1388,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1380,7 +1411,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1402,8 +1433,12 @@
       <c r="G44">
         <v>60</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <f>(AVERAGE(E44:E47) - AVERAGE(E48:E49)) * 60/AVERAGE(G44:G47)</f>
+        <v>1.9834710743801653</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1426,7 +1461,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1449,7 +1484,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1472,7 +1507,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1495,7 +1530,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1518,7 +1553,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1540,8 +1575,12 @@
       <c r="G50">
         <v>61</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <f>(AVERAGE(E50, E52:E53) - AVERAGE(E54:E55)) * 60/AVERAGE(G50:G53)</f>
+        <v>21.322314049586776</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1564,7 +1603,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1587,7 +1626,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1610,7 +1649,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1633,7 +1672,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1656,7 +1695,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1678,8 +1717,12 @@
       <c r="G56">
         <v>60</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56">
+        <f>(AVERAGE(E56:E59) - AVERAGE(E60:E61)) * 60/AVERAGE(G56:G59)</f>
+        <v>13.25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1702,7 +1745,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1725,7 +1768,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1748,7 +1791,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1771,7 +1814,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1794,7 +1837,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1816,8 +1859,12 @@
       <c r="G62">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62">
+        <f>(AVERAGE(E62:E65) - AVERAGE(E66:E67)) * 60/AVERAGE(G62:G65)</f>
+        <v>-13.75</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1840,7 +1887,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1863,7 +1910,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1886,7 +1933,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1909,7 +1956,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1932,7 +1979,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1954,8 +2001,12 @@
       <c r="G68">
         <v>60</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H68">
+        <f>(AVERAGE(E69:E71) - AVERAGE(E72:E73)) * 60/AVERAGE(G68:G71)</f>
+        <v>16.333333333333336</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1978,7 +2029,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2001,7 +2052,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2024,7 +2075,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2047,7 +2098,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2070,7 +2121,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2092,8 +2143,12 @@
       <c r="G74">
         <v>60</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H74">
+        <f>(AVERAGE(E74:E76) - AVERAGE(E78:E79)) * 60/AVERAGE(G74:G76)</f>
+        <v>8.5474860335195526</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2116,7 +2171,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2139,7 +2194,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2162,7 +2217,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2185,7 +2240,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2208,7 +2263,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2230,8 +2285,12 @@
       <c r="G80">
         <v>60</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H80">
+        <f>(AVERAGE(E80:E83) - AVERAGE(E84:E85)) * 60/AVERAGE(G80:G83)</f>
+        <v>19.25</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2254,7 +2313,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2277,7 +2336,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2300,7 +2359,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2323,7 +2382,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2346,7 +2405,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2368,8 +2427,12 @@
       <c r="G86">
         <v>60</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H86">
+        <f>(AVERAGE(E86:E89) - AVERAGE(E90:E91)) * 60/AVERAGE(G86:G89)</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2392,7 +2455,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2415,7 +2478,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2438,7 +2501,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2461,7 +2524,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2484,7 +2547,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2506,8 +2569,12 @@
       <c r="G92">
         <v>60</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H92">
+        <f>(AVERAGE(E92:E95) - AVERAGE(E96:E97)) * 60/AVERAGE(G92:G95)</f>
+        <v>25.25</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2530,7 +2597,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2553,7 +2620,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2576,7 +2643,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2599,7 +2666,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2622,7 +2689,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2644,8 +2711,12 @@
       <c r="G98">
         <v>60</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H98">
+        <f>(AVERAGE(E98:E101) - AVERAGE(E102:E103)) * 60/AVERAGE(G98:G101)</f>
+        <v>70.292887029288707</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2668,7 +2739,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2691,7 +2762,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2714,7 +2785,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2737,7 +2808,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2760,7 +2831,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2782,8 +2853,12 @@
       <c r="G104">
         <v>60</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H104">
+        <f>(AVERAGE(E104:E107) - AVERAGE(E108:E109)) * 60/AVERAGE(G104:G107)</f>
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2806,7 +2881,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2829,7 +2904,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2852,7 +2927,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2875,7 +2950,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2898,7 +2973,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -2920,8 +2995,12 @@
       <c r="G110">
         <v>60</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H110">
+        <f>(AVERAGE(E110:E113) - AVERAGE(E114:E115)) * 60/AVERAGE(G110:G113)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -2944,7 +3023,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -2967,7 +3046,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -2990,7 +3069,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -3013,7 +3092,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -3036,7 +3115,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -3058,8 +3137,12 @@
       <c r="G116">
         <v>60</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H116">
+        <f>(AVERAGE(E116:E119) - AVERAGE(E120:E121)) * 60/AVERAGE(G116:G119)</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -3082,7 +3165,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -3105,7 +3188,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -3128,7 +3211,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -3151,7 +3234,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -3174,7 +3257,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -3196,8 +3279,12 @@
       <c r="G122">
         <v>60</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H122">
+        <f>(AVERAGE(E122:E125) - AVERAGE(E126:E127)) * 60/AVERAGE(G122:G125)</f>
+        <v>97.815126050420162</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -3220,7 +3307,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -3243,7 +3330,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -3266,7 +3353,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -3289,7 +3376,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -3312,7 +3399,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -3334,8 +3421,12 @@
       <c r="G128">
         <v>320</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H128">
+        <f>(AVERAGE(E128:E131) - AVERAGE(E132:E133)) * 60/AVERAGE(G128:G131)</f>
+        <v>34.620797498045349</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -3358,7 +3449,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -3381,7 +3472,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -3404,7 +3495,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -3427,7 +3518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -3450,7 +3541,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -3472,8 +3563,12 @@
       <c r="G134">
         <v>60</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H134">
+        <f>(AVERAGE(E134:E137) - AVERAGE(E138:E139)) * 60/AVERAGE(G134:G137)</f>
+        <v>17.25</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -3496,7 +3591,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -3519,7 +3614,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -3542,7 +3637,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -3565,7 +3660,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -3588,7 +3683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>1</v>
       </c>
@@ -3607,8 +3702,12 @@
       <c r="G140">
         <v>60</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H140">
+        <f>(AVERAGE(E140:E143) - AVERAGE(E144:E145)) * 60/AVERAGE(G140:G143)</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>2</v>
       </c>
@@ -3628,7 +3727,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>3</v>
       </c>
@@ -3648,7 +3747,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>4</v>
       </c>
@@ -3668,7 +3767,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>5</v>
       </c>
@@ -3688,7 +3787,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>6</v>
       </c>
@@ -3708,7 +3807,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>7</v>
       </c>
@@ -3727,8 +3826,12 @@
       <c r="G146">
         <v>65</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H146">
+        <f>(AVERAGE(E146:E149) - AVERAGE(E150:E151)) * 60/AVERAGE(G146:G149)</f>
+        <v>26.76923076923077</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>8</v>
       </c>
@@ -3748,7 +3851,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>9</v>
       </c>
@@ -3768,7 +3871,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>10</v>
       </c>
@@ -3788,7 +3891,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>11</v>
       </c>
@@ -3808,7 +3911,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>12</v>
       </c>
@@ -3828,7 +3931,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>13</v>
       </c>
@@ -3847,8 +3950,12 @@
       <c r="G152">
         <v>60</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H152">
+        <f>(AVERAGE(E152:E155) - AVERAGE(E156:E157)) * 60/AVERAGE(G152:G155)</f>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>14</v>
       </c>
@@ -3868,7 +3975,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>15</v>
       </c>
@@ -3888,7 +3995,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>16</v>
       </c>
@@ -3908,7 +4015,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>17</v>
       </c>
@@ -3928,7 +4035,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>18</v>
       </c>
@@ -3948,7 +4055,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>19</v>
       </c>
@@ -3967,8 +4074,12 @@
       <c r="G158">
         <v>60</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H158">
+        <f>(AVERAGE(E158:E161) - AVERAGE(E162:E163)) * 60/AVERAGE(G158:G161)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>20</v>
       </c>
@@ -3988,7 +4099,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>21</v>
       </c>
@@ -4008,7 +4119,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>22</v>
       </c>
@@ -4028,7 +4139,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>23</v>
       </c>
@@ -4048,7 +4159,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>24</v>
       </c>
@@ -4068,7 +4179,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>25</v>
       </c>
@@ -4087,8 +4198,12 @@
       <c r="G164">
         <v>60</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H164">
+        <f>(AVERAGE(E164:E167) - AVERAGE(E168:E169)) * 60/AVERAGE(G164:G167)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>26</v>
       </c>
@@ -4108,7 +4223,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>27</v>
       </c>
@@ -4128,7 +4243,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>28</v>
       </c>
@@ -4148,7 +4263,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>29</v>
       </c>
@@ -4168,7 +4283,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>30</v>
       </c>
@@ -4188,7 +4303,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>31</v>
       </c>
@@ -4207,8 +4322,12 @@
       <c r="G170">
         <v>60</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H170">
+        <f>(AVERAGE(E170:E173) - AVERAGE(E174:E175)) * 60/AVERAGE(G170:G173)</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>32</v>
       </c>
@@ -4228,7 +4347,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>33</v>
       </c>
@@ -4248,7 +4367,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>34</v>
       </c>
@@ -4268,7 +4387,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>35</v>
       </c>
@@ -4288,7 +4407,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>36</v>
       </c>
@@ -4308,7 +4427,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>37</v>
       </c>
@@ -4327,8 +4446,12 @@
       <c r="G176">
         <v>67</v>
       </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H176">
+        <f>(AVERAGE(E176:E179) - AVERAGE(E180:E181)) * 60/AVERAGE(G176:G179)</f>
+        <v>147.95454545454547</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>38</v>
       </c>
@@ -4348,7 +4471,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>39</v>
       </c>
@@ -4368,7 +4491,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>40</v>
       </c>
@@ -4388,7 +4511,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>41</v>
       </c>
@@ -4408,7 +4531,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>42</v>
       </c>
@@ -4428,7 +4551,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>43</v>
       </c>
@@ -4447,8 +4570,12 @@
       <c r="G182">
         <v>60</v>
       </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H182">
+        <f>(AVERAGE(E182:E185) - AVERAGE(E186:E187)) * 60/AVERAGE(G182:G185)</f>
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>44</v>
       </c>
@@ -4468,7 +4595,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>45</v>
       </c>
@@ -4488,7 +4615,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>46</v>
       </c>
@@ -4508,7 +4635,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>47</v>
       </c>
@@ -4528,7 +4655,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>48</v>
       </c>
@@ -4548,7 +4675,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>49</v>
       </c>
@@ -4567,8 +4694,12 @@
       <c r="G188">
         <v>56</v>
       </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H188">
+        <f>(AVERAGE(E188:E191) - AVERAGE(E192:E193)) * 60/AVERAGE(G188:G191)</f>
+        <v>36.942148760330582</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>50</v>
       </c>
@@ -4588,7 +4719,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>51</v>
       </c>
@@ -4608,7 +4739,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>52</v>
       </c>
@@ -4628,7 +4759,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>53</v>
       </c>
@@ -4648,7 +4779,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>54</v>
       </c>
@@ -4668,7 +4799,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>55</v>
       </c>
@@ -4687,8 +4818,12 @@
       <c r="G194">
         <v>61</v>
       </c>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H194">
+        <f>(AVERAGE(E194:E197) - AVERAGE(E198:E199)) * 60/AVERAGE(G194:G197)</f>
+        <v>132.04918032786884</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>56</v>
       </c>
@@ -4708,7 +4843,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>57</v>
       </c>
@@ -4728,7 +4863,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>58</v>
       </c>
@@ -4748,7 +4883,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>59</v>
       </c>
@@ -4768,7 +4903,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>60</v>
       </c>
@@ -4788,7 +4923,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>61</v>
       </c>
@@ -4807,8 +4942,12 @@
       <c r="G200">
         <v>60</v>
       </c>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H200">
+        <f>(AVERAGE(E200:E203) - AVERAGE(E204:E205)) * 60/AVERAGE(G200:G203)</f>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>62</v>
       </c>
@@ -4828,7 +4967,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>63</v>
       </c>
@@ -4848,7 +4987,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>64</v>
       </c>
@@ -4868,7 +5007,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>65</v>
       </c>
@@ -4888,7 +5027,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>66</v>
       </c>
@@ -4908,7 +5047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>67</v>
       </c>
@@ -4927,8 +5066,12 @@
       <c r="G206">
         <v>60</v>
       </c>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H206">
+        <f>(AVERAGE(E206:E209) - AVERAGE(E210:E211)) * 60/AVERAGE(G206:G209)</f>
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>68</v>
       </c>
@@ -4948,7 +5091,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>69</v>
       </c>

</xml_diff>